<commit_message>
update localization files to contain dutch translations, red = unconfirmed translations Update SUGAR Prefabs to have the localization components
</commit_message>
<xml_diff>
--- a/Assets/Resources/Localization/SMILocalization.xlsx
+++ b/Assets/Resources/Localization/SMILocalization.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="130">
   <si>
     <t>Key</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Close</t>
-  </si>
-  <si>
-    <t>XXXX</t>
   </si>
   <si>
     <t>COMMENT_NEGATIVE</t>
@@ -396,6 +393,24 @@
   </si>
   <si>
     <t>Informeren</t>
+  </si>
+  <si>
+    <t>Pagina {0}</t>
+  </si>
+  <si>
+    <t>Naburig</t>
+  </si>
+  <si>
+    <t>Nabij</t>
+  </si>
+  <si>
+    <t>Uitgang</t>
+  </si>
+  <si>
+    <t>Voorgaand</t>
+  </si>
+  <si>
+    <t>Vrienden</t>
   </si>
 </sst>
 </file>
@@ -734,7 +749,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -913,7 +928,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -926,13 +941,13 @@
     </row>
     <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -945,13 +960,13 @@
     </row>
     <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -964,13 +979,13 @@
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -983,13 +998,13 @@
     </row>
     <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1002,13 +1017,13 @@
     </row>
     <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1021,13 +1036,13 @@
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1040,13 +1055,13 @@
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1059,13 +1074,13 @@
     </row>
     <row r="17" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1078,13 +1093,13 @@
     </row>
     <row r="18" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1097,13 +1112,13 @@
     </row>
     <row r="19" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C19" s="4" t="s">
-        <v>23</v>
+        <v>129</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1116,13 +1131,13 @@
     </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1135,13 +1150,13 @@
     </row>
     <row r="21" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1154,13 +1169,13 @@
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1173,13 +1188,13 @@
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1192,13 +1207,13 @@
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1211,13 +1226,13 @@
     </row>
     <row r="25" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1230,13 +1245,13 @@
     </row>
     <row r="26" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1264,13 +1279,13 @@
     </row>
     <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1283,13 +1298,13 @@
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1302,13 +1317,13 @@
     </row>
     <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1321,13 +1336,13 @@
     </row>
     <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1340,13 +1355,13 @@
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1359,13 +1374,13 @@
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="C32" s="4" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1378,13 +1393,13 @@
     </row>
     <row r="33" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1397,13 +1412,13 @@
     </row>
     <row r="34" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="C34" s="4" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1416,13 +1431,13 @@
     </row>
     <row r="35" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1435,13 +1450,13 @@
     </row>
     <row r="36" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1454,13 +1469,13 @@
     </row>
     <row r="37" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1473,13 +1488,13 @@
     </row>
     <row r="38" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1492,13 +1507,13 @@
     </row>
     <row r="39" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1511,13 +1526,13 @@
     </row>
     <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1530,13 +1545,13 @@
     </row>
     <row r="41" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="C41" s="4" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1549,13 +1564,13 @@
     </row>
     <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C42" s="4" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1568,13 +1583,13 @@
     </row>
     <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1587,13 +1602,13 @@
     </row>
     <row r="44" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1606,13 +1621,13 @@
     </row>
     <row r="45" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1625,13 +1640,13 @@
     </row>
     <row r="46" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1644,13 +1659,13 @@
     </row>
     <row r="47" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>

</xml_diff>